<commit_message>
Modified TrainSets, Trains, added Compartments in database
</commit_message>
<xml_diff>
--- a/System_Biletow/cars-and-seats.xlsx
+++ b/System_Biletow/cars-and-seats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marta\source\repos\System_Biletow\System_Biletow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A68D9A50-9A2B-4935-9467-07E735A0BA9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38B949AD-8E90-4B77-83C6-67734D51BB15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28905" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="2" xr2:uid="{0AE42409-A18E-481D-BAD6-AC22FA644729}"/>
+    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="11370" activeTab="1" xr2:uid="{0AE42409-A18E-481D-BAD6-AC22FA644729}"/>
   </bookViews>
   <sheets>
     <sheet name="TrainSets" sheetId="1" r:id="rId1"/>
@@ -473,13 +473,13 @@
       <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -490,7 +490,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>18</v>
       </c>
@@ -498,19 +498,19 @@
         <v>2</v>
       </c>
       <c r="C2" t="str">
-        <f>_xlfn.CONCAT("(6, ",$C$1,"IC 3806/7",$C$1,", ")</f>
-        <v xml:space="preserve">(6, "IC 3806/7", </v>
+        <f>_xlfn.CONCAT("(2, ",$C$1,"IC 8306/7",$C$1,", ")</f>
+        <v xml:space="preserve">(2, "IC 8306/7", </v>
       </c>
       <c r="D2" t="str">
         <f>_xlfn.CONCAT(C2,$C$1,B2,$C$1,", ")</f>
-        <v xml:space="preserve">(6, "IC 3806/7", "B10nouz", </v>
+        <v xml:space="preserve">(2, "IC 8306/7", "B10nouz", </v>
       </c>
       <c r="E2" t="str">
         <f>_xlfn.CONCAT(D2,A2,"), ")</f>
-        <v xml:space="preserve">(6, "IC 3806/7", "B10nouz", 18), </v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">(2, "IC 8306/7", "B10nouz", 18), </v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>17</v>
       </c>
@@ -518,19 +518,19 @@
         <v>3</v>
       </c>
       <c r="C3" t="str">
-        <f t="shared" ref="C3:C9" si="0">_xlfn.CONCAT("(6, ",$C$1,"IC 3806/7",$C$1,", ")</f>
-        <v xml:space="preserve">(6, "IC 3806/7", </v>
+        <f t="shared" ref="C3:C9" si="0">_xlfn.CONCAT("(2, ",$C$1,"IC 8306/7",$C$1,", ")</f>
+        <v xml:space="preserve">(2, "IC 8306/7", </v>
       </c>
       <c r="D3" t="str">
         <f t="shared" ref="D3:D9" si="1">_xlfn.CONCAT(C3,$C$1,B3,$C$1,", ")</f>
-        <v xml:space="preserve">(6, "IC 3806/7", "B9nopuvz", </v>
+        <v xml:space="preserve">(2, "IC 8306/7", "B9nopuvz", </v>
       </c>
       <c r="E3" t="str">
         <f t="shared" ref="E3:E9" si="2">_xlfn.CONCAT(D3,A3,"), ")</f>
-        <v xml:space="preserve">(6, "IC 3806/7", "B9nopuvz", 17), </v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">(2, "IC 8306/7", "B9nopuvz", 17), </v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>16</v>
       </c>
@@ -539,18 +539,18 @@
       </c>
       <c r="C4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">(6, "IC 3806/7", </v>
+        <v xml:space="preserve">(2, "IC 8306/7", </v>
       </c>
       <c r="D4" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">(6, "IC 3806/7", "B9nopuz", </v>
+        <v xml:space="preserve">(2, "IC 8306/7", "B9nopuz", </v>
       </c>
       <c r="E4" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">(6, "IC 3806/7", "B9nopuz", 16), </v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">(2, "IC 8306/7", "B9nopuz", 16), </v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>15</v>
       </c>
@@ -559,18 +559,18 @@
       </c>
       <c r="C5" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">(6, "IC 3806/7", </v>
+        <v xml:space="preserve">(2, "IC 8306/7", </v>
       </c>
       <c r="D5" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">(6, "IC 3806/7", "B9nopuz", </v>
+        <v xml:space="preserve">(2, "IC 8306/7", "B9nopuz", </v>
       </c>
       <c r="E5" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">(6, "IC 3806/7", "B9nopuz", 15), </v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">(2, "IC 8306/7", "B9nopuz", 15), </v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>14</v>
       </c>
@@ -579,18 +579,18 @@
       </c>
       <c r="C6" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">(6, "IC 3806/7", </v>
+        <v xml:space="preserve">(2, "IC 8306/7", </v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">(6, "IC 3806/7", "B10nouz", </v>
+        <v xml:space="preserve">(2, "IC 8306/7", "B10nouz", </v>
       </c>
       <c r="E6" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">(6, "IC 3806/7", "B10nouz", 14), </v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">(2, "IC 8306/7", "B10nouz", 14), </v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>13</v>
       </c>
@@ -599,18 +599,18 @@
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">(6, "IC 3806/7", </v>
+        <v xml:space="preserve">(2, "IC 8306/7", </v>
       </c>
       <c r="D7" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">(6, "IC 3806/7", "B7bnopuz", </v>
+        <v xml:space="preserve">(2, "IC 8306/7", "B7bnopuz", </v>
       </c>
       <c r="E7" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">(6, "IC 3806/7", "B7bnopuz", 13), </v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">(2, "IC 8306/7", "B7bnopuz", 13), </v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>12</v>
       </c>
@@ -619,18 +619,18 @@
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">(6, "IC 3806/7", </v>
+        <v xml:space="preserve">(2, "IC 8306/7", </v>
       </c>
       <c r="D8" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">(6, "IC 3806/7", "WRnouz", </v>
+        <v xml:space="preserve">(2, "IC 8306/7", "WRnouz", </v>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">(6, "IC 3806/7", "WRnouz", 12), </v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">(2, "IC 8306/7", "WRnouz", 12), </v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>11</v>
       </c>
@@ -639,15 +639,15 @@
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">(6, "IC 3806/7", </v>
+        <v xml:space="preserve">(2, "IC 8306/7", </v>
       </c>
       <c r="D9" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">(6, "IC 3806/7", "A9nouz", </v>
+        <v xml:space="preserve">(2, "IC 8306/7", "A9nouz", </v>
       </c>
       <c r="E9" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">(6, "IC 3806/7", "A9nouz", 11), </v>
+        <v xml:space="preserve">(2, "IC 8306/7", "A9nouz", 11), </v>
       </c>
     </row>
   </sheetData>
@@ -659,16 +659,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C9B2C30-95FD-4C71-961A-ECB353A345A8}">
   <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:L1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="8" max="8" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="0" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="4.7265625" hidden="1" customWidth="1"/>
+    <col min="9" max="11" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -694,7 +696,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>11</v>
       </c>
@@ -724,7 +726,7 @@
         <v xml:space="preserve">(11, "B10nouz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>12</v>
       </c>
@@ -754,7 +756,7 @@
         <v xml:space="preserve">(12, "B10nouz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>13</v>
       </c>
@@ -784,7 +786,7 @@
         <v xml:space="preserve">(13, "B10nouz", 0, 1, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>14</v>
       </c>
@@ -814,7 +816,7 @@
         <v xml:space="preserve">(14, "B10nouz", 0, 1, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>15</v>
       </c>
@@ -844,7 +846,7 @@
         <v xml:space="preserve">(15, "B10nouz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>16</v>
       </c>
@@ -874,7 +876,7 @@
         <v xml:space="preserve">(16, "B10nouz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>21</v>
       </c>
@@ -904,7 +906,7 @@
         <v xml:space="preserve">(21, "B10nouz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>22</v>
       </c>
@@ -934,7 +936,7 @@
         <v xml:space="preserve">(22, "B10nouz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>23</v>
       </c>
@@ -964,7 +966,7 @@
         <v xml:space="preserve">(23, "B10nouz", 0, 1, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>24</v>
       </c>
@@ -994,7 +996,7 @@
         <v xml:space="preserve">(24, "B10nouz", 0, 1, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>25</v>
       </c>
@@ -1024,7 +1026,7 @@
         <v xml:space="preserve">(25, "B10nouz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>26</v>
       </c>
@@ -1054,7 +1056,7 @@
         <v xml:space="preserve">(26, "B10nouz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>31</v>
       </c>
@@ -1084,7 +1086,7 @@
         <v xml:space="preserve">(31, "B10nouz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>32</v>
       </c>
@@ -1114,7 +1116,7 @@
         <v xml:space="preserve">(32, "B10nouz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>33</v>
       </c>
@@ -1144,7 +1146,7 @@
         <v xml:space="preserve">(33, "B10nouz", 0, 1, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>34</v>
       </c>
@@ -1174,7 +1176,7 @@
         <v xml:space="preserve">(34, "B10nouz", 0, 1, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>35</v>
       </c>
@@ -1204,7 +1206,7 @@
         <v xml:space="preserve">(35, "B10nouz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>36</v>
       </c>
@@ -1234,7 +1236,7 @@
         <v xml:space="preserve">(36, "B10nouz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>41</v>
       </c>
@@ -1264,7 +1266,7 @@
         <v xml:space="preserve">(41, "B10nouz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>42</v>
       </c>
@@ -1294,7 +1296,7 @@
         <v xml:space="preserve">(42, "B10nouz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>43</v>
       </c>
@@ -1324,7 +1326,7 @@
         <v xml:space="preserve">(43, "B10nouz", 0, 1, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>44</v>
       </c>
@@ -1354,7 +1356,7 @@
         <v xml:space="preserve">(44, "B10nouz", 0, 1, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>45</v>
       </c>
@@ -1384,7 +1386,7 @@
         <v xml:space="preserve">(45, "B10nouz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>46</v>
       </c>
@@ -1414,7 +1416,7 @@
         <v xml:space="preserve">(46, "B10nouz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>51</v>
       </c>
@@ -1444,7 +1446,7 @@
         <v xml:space="preserve">(51, "B10nouz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>52</v>
       </c>
@@ -1474,7 +1476,7 @@
         <v xml:space="preserve">(52, "B10nouz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>53</v>
       </c>
@@ -1504,7 +1506,7 @@
         <v xml:space="preserve">(53, "B10nouz", 0, 1, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>54</v>
       </c>
@@ -1534,7 +1536,7 @@
         <v xml:space="preserve">(54, "B10nouz", 0, 1, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>55</v>
       </c>
@@ -1564,7 +1566,7 @@
         <v xml:space="preserve">(55, "B10nouz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>56</v>
       </c>
@@ -1594,7 +1596,7 @@
         <v xml:space="preserve">(56, "B10nouz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>61</v>
       </c>
@@ -1624,7 +1626,7 @@
         <v xml:space="preserve">(61, "B10nouz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>62</v>
       </c>
@@ -1654,7 +1656,7 @@
         <v xml:space="preserve">(62, "B10nouz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>63</v>
       </c>
@@ -1684,7 +1686,7 @@
         <v xml:space="preserve">(63, "B10nouz", 0, 1, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>64</v>
       </c>
@@ -1714,7 +1716,7 @@
         <v xml:space="preserve">(64, "B10nouz", 0, 1, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>65</v>
       </c>
@@ -1744,7 +1746,7 @@
         <v xml:space="preserve">(65, "B10nouz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>66</v>
       </c>
@@ -1774,7 +1776,7 @@
         <v xml:space="preserve">(66, "B10nouz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>71</v>
       </c>
@@ -1804,7 +1806,7 @@
         <v xml:space="preserve">(71, "B10nouz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>72</v>
       </c>
@@ -1834,7 +1836,7 @@
         <v xml:space="preserve">(72, "B10nouz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>73</v>
       </c>
@@ -1864,7 +1866,7 @@
         <v xml:space="preserve">(73, "B10nouz", 0, 1, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>74</v>
       </c>
@@ -1894,7 +1896,7 @@
         <v xml:space="preserve">(74, "B10nouz", 0, 1, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>75</v>
       </c>
@@ -1924,7 +1926,7 @@
         <v xml:space="preserve">(75, "B10nouz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>76</v>
       </c>
@@ -1954,7 +1956,7 @@
         <v xml:space="preserve">(76, "B10nouz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>81</v>
       </c>
@@ -1984,7 +1986,7 @@
         <v xml:space="preserve">(81, "B10nouz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>82</v>
       </c>
@@ -2014,7 +2016,7 @@
         <v xml:space="preserve">(82, "B10nouz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>83</v>
       </c>
@@ -2044,7 +2046,7 @@
         <v xml:space="preserve">(83, "B10nouz", 0, 1, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>84</v>
       </c>
@@ -2074,7 +2076,7 @@
         <v xml:space="preserve">(84, "B10nouz", 0, 1, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>85</v>
       </c>
@@ -2104,7 +2106,7 @@
         <v xml:space="preserve">(85, "B10nouz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>86</v>
       </c>
@@ -2134,7 +2136,7 @@
         <v xml:space="preserve">(86, "B10nouz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>91</v>
       </c>
@@ -2164,7 +2166,7 @@
         <v xml:space="preserve">(91, "B10nouz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>92</v>
       </c>
@@ -2194,7 +2196,7 @@
         <v xml:space="preserve">(92, "B10nouz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>93</v>
       </c>
@@ -2224,7 +2226,7 @@
         <v xml:space="preserve">(93, "B10nouz", 0, 1, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>94</v>
       </c>
@@ -2254,7 +2256,7 @@
         <v xml:space="preserve">(94, "B10nouz", 0, 1, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>95</v>
       </c>
@@ -2284,7 +2286,7 @@
         <v xml:space="preserve">(95, "B10nouz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>96</v>
       </c>
@@ -2314,7 +2316,7 @@
         <v xml:space="preserve">(96, "B10nouz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>101</v>
       </c>
@@ -2344,7 +2346,7 @@
         <v xml:space="preserve">(101, "B10nouz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>102</v>
       </c>
@@ -2374,7 +2376,7 @@
         <v xml:space="preserve">(102, "B10nouz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>103</v>
       </c>
@@ -2404,7 +2406,7 @@
         <v xml:space="preserve">(103, "B10nouz", 0, 1, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>104</v>
       </c>
@@ -2434,7 +2436,7 @@
         <v xml:space="preserve">(104, "B10nouz", 0, 1, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>105</v>
       </c>
@@ -2464,7 +2466,7 @@
         <v xml:space="preserve">(105, "B10nouz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>106</v>
       </c>
@@ -2503,16 +2505,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A768BC9D-EB04-4FCF-8809-241C38D14EA7}">
   <dimension ref="A1:K73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+    <sheetView topLeftCell="A52" workbookViewId="0">
       <selection activeCell="K58" sqref="K58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="8" max="8" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -2538,7 +2540,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>11</v>
       </c>
@@ -2572,7 +2574,7 @@
         <v xml:space="preserve">(11, "B9nopuvz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>12</v>
       </c>
@@ -2603,7 +2605,7 @@
         <v xml:space="preserve">(12, "B9nopuvz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>13</v>
       </c>
@@ -2637,7 +2639,7 @@
         <v xml:space="preserve">(13, "B9nopuvz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>14</v>
       </c>
@@ -2668,7 +2670,7 @@
         <v xml:space="preserve">(14, "B9nopuvz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>15</v>
       </c>
@@ -2699,7 +2701,7 @@
         <v xml:space="preserve">(15, "B9nopuvz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>16</v>
       </c>
@@ -2730,7 +2732,7 @@
         <v xml:space="preserve">(16, "B9nopuvz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>17</v>
       </c>
@@ -2761,7 +2763,7 @@
         <v xml:space="preserve">(17, "B9nopuvz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>18</v>
       </c>
@@ -2795,7 +2797,7 @@
         <v xml:space="preserve">(18, "B9nopuvz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>21</v>
       </c>
@@ -2826,7 +2828,7 @@
         <v xml:space="preserve">(21, "B9nopuvz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>22</v>
       </c>
@@ -2857,7 +2859,7 @@
         <v xml:space="preserve">(22, "B9nopuvz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>23</v>
       </c>
@@ -2888,7 +2890,7 @@
         <v xml:space="preserve">(23, "B9nopuvz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>24</v>
       </c>
@@ -2919,7 +2921,7 @@
         <v xml:space="preserve">(24, "B9nopuvz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>25</v>
       </c>
@@ -2950,7 +2952,7 @@
         <v xml:space="preserve">(25, "B9nopuvz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>26</v>
       </c>
@@ -2981,7 +2983,7 @@
         <v xml:space="preserve">(26, "B9nopuvz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>27</v>
       </c>
@@ -3012,7 +3014,7 @@
         <v xml:space="preserve">(27, "B9nopuvz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>28</v>
       </c>
@@ -3043,7 +3045,7 @@
         <v xml:space="preserve">(28, "B9nopuvz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>31</v>
       </c>
@@ -3074,7 +3076,7 @@
         <v xml:space="preserve">(31, "B9nopuvz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>32</v>
       </c>
@@ -3105,7 +3107,7 @@
         <v xml:space="preserve">(32, "B9nopuvz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>33</v>
       </c>
@@ -3136,7 +3138,7 @@
         <v xml:space="preserve">(33, "B9nopuvz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>34</v>
       </c>
@@ -3167,7 +3169,7 @@
         <v xml:space="preserve">(34, "B9nopuvz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>35</v>
       </c>
@@ -3198,7 +3200,7 @@
         <v xml:space="preserve">(35, "B9nopuvz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>36</v>
       </c>
@@ -3229,7 +3231,7 @@
         <v xml:space="preserve">(36, "B9nopuvz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>37</v>
       </c>
@@ -3260,7 +3262,7 @@
         <v xml:space="preserve">(37, "B9nopuvz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>38</v>
       </c>
@@ -3291,7 +3293,7 @@
         <v xml:space="preserve">(38, "B9nopuvz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>41</v>
       </c>
@@ -3322,7 +3324,7 @@
         <v xml:space="preserve">(41, "B9nopuvz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>42</v>
       </c>
@@ -3353,7 +3355,7 @@
         <v xml:space="preserve">(42, "B9nopuvz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>43</v>
       </c>
@@ -3384,7 +3386,7 @@
         <v xml:space="preserve">(43, "B9nopuvz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>44</v>
       </c>
@@ -3415,7 +3417,7 @@
         <v xml:space="preserve">(44, "B9nopuvz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>45</v>
       </c>
@@ -3446,7 +3448,7 @@
         <v xml:space="preserve">(45, "B9nopuvz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>46</v>
       </c>
@@ -3477,7 +3479,7 @@
         <v xml:space="preserve">(46, "B9nopuvz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>47</v>
       </c>
@@ -3508,7 +3510,7 @@
         <v xml:space="preserve">(47, "B9nopuvz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>48</v>
       </c>
@@ -3539,7 +3541,7 @@
         <v xml:space="preserve">(48, "B9nopuvz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>51</v>
       </c>
@@ -3570,7 +3572,7 @@
         <v xml:space="preserve">(51, "B9nopuvz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>52</v>
       </c>
@@ -3601,7 +3603,7 @@
         <v xml:space="preserve">(52, "B9nopuvz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>53</v>
       </c>
@@ -3632,7 +3634,7 @@
         <v xml:space="preserve">(53, "B9nopuvz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>54</v>
       </c>
@@ -3663,7 +3665,7 @@
         <v xml:space="preserve">(54, "B9nopuvz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>55</v>
       </c>
@@ -3694,7 +3696,7 @@
         <v xml:space="preserve">(55, "B9nopuvz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>56</v>
       </c>
@@ -3725,7 +3727,7 @@
         <v xml:space="preserve">(56, "B9nopuvz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>57</v>
       </c>
@@ -3756,7 +3758,7 @@
         <v xml:space="preserve">(57, "B9nopuvz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>58</v>
       </c>
@@ -3787,7 +3789,7 @@
         <v xml:space="preserve">(58, "B9nopuvz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>61</v>
       </c>
@@ -3818,7 +3820,7 @@
         <v xml:space="preserve">(61, "B9nopuvz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>62</v>
       </c>
@@ -3849,7 +3851,7 @@
         <v xml:space="preserve">(62, "B9nopuvz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>63</v>
       </c>
@@ -3880,7 +3882,7 @@
         <v xml:space="preserve">(63, "B9nopuvz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>64</v>
       </c>
@@ -3911,7 +3913,7 @@
         <v xml:space="preserve">(64, "B9nopuvz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>65</v>
       </c>
@@ -3942,7 +3944,7 @@
         <v xml:space="preserve">(65, "B9nopuvz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>66</v>
       </c>
@@ -3973,7 +3975,7 @@
         <v xml:space="preserve">(66, "B9nopuvz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>67</v>
       </c>
@@ -4004,7 +4006,7 @@
         <v xml:space="preserve">(67, "B9nopuvz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>68</v>
       </c>
@@ -4035,7 +4037,7 @@
         <v xml:space="preserve">(68, "B9nopuvz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>71</v>
       </c>
@@ -4066,7 +4068,7 @@
         <v xml:space="preserve">(71, "B9nopuvz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>72</v>
       </c>
@@ -4097,7 +4099,7 @@
         <v xml:space="preserve">(72, "B9nopuvz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>73</v>
       </c>
@@ -4128,7 +4130,7 @@
         <v xml:space="preserve">(73, "B9nopuvz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>74</v>
       </c>
@@ -4159,7 +4161,7 @@
         <v xml:space="preserve">(74, "B9nopuvz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>75</v>
       </c>
@@ -4190,7 +4192,7 @@
         <v xml:space="preserve">(75, "B9nopuvz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>76</v>
       </c>
@@ -4221,7 +4223,7 @@
         <v xml:space="preserve">(76, "B9nopuvz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>77</v>
       </c>
@@ -4252,7 +4254,7 @@
         <v xml:space="preserve">(77, "B9nopuvz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>78</v>
       </c>
@@ -4283,7 +4285,7 @@
         <v xml:space="preserve">(78, "B9nopuvz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>81</v>
       </c>
@@ -4314,7 +4316,7 @@
         <v xml:space="preserve">(81, "B9nopuvz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>82</v>
       </c>
@@ -4345,7 +4347,7 @@
         <v xml:space="preserve">(82, "B9nopuvz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>83</v>
       </c>
@@ -4376,7 +4378,7 @@
         <v xml:space="preserve">(83, "B9nopuvz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>84</v>
       </c>
@@ -4410,7 +4412,7 @@
         <v xml:space="preserve">(84, "B9nopuvz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>85</v>
       </c>
@@ -4441,7 +4443,7 @@
         <v xml:space="preserve">(85, "B9nopuvz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>86</v>
       </c>
@@ -4472,7 +4474,7 @@
         <v xml:space="preserve">(86, "B9nopuvz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>87</v>
       </c>
@@ -4503,7 +4505,7 @@
         <v xml:space="preserve">(87, "B9nopuvz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>88</v>
       </c>
@@ -4534,7 +4536,7 @@
         <v xml:space="preserve">(88, "B9nopuvz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>91</v>
       </c>
@@ -4565,7 +4567,7 @@
         <v xml:space="preserve">(91, "B9nopuvz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>92</v>
       </c>
@@ -4596,7 +4598,7 @@
         <v xml:space="preserve">(92, "B9nopuvz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>93</v>
       </c>
@@ -4627,7 +4629,7 @@
         <v xml:space="preserve">(93, "B9nopuvz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>94</v>
       </c>
@@ -4658,7 +4660,7 @@
         <v xml:space="preserve">(94, "B9nopuvz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>95</v>
       </c>
@@ -4692,7 +4694,7 @@
         <v xml:space="preserve">(95, "B9nopuvz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>96</v>
       </c>
@@ -4723,7 +4725,7 @@
         <v xml:space="preserve">(96, "B9nopuvz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>97</v>
       </c>
@@ -4757,7 +4759,7 @@
         <v xml:space="preserve">(97, "B9nopuvz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>98</v>
       </c>
@@ -4801,12 +4803,12 @@
       <selection activeCell="L1" sqref="L1:L1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="8" max="8" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -4832,7 +4834,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>11</v>
       </c>
@@ -4870,7 +4872,7 @@
         <v xml:space="preserve">(11, "B9nopuz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>12</v>
       </c>
@@ -4908,7 +4910,7 @@
         <v xml:space="preserve">(12, "B9nopuz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>13</v>
       </c>
@@ -4946,7 +4948,7 @@
         <v xml:space="preserve">(13, "B9nopuz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>14</v>
       </c>
@@ -4984,7 +4986,7 @@
         <v xml:space="preserve">(14, "B9nopuz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>15</v>
       </c>
@@ -5022,7 +5024,7 @@
         <v xml:space="preserve">(15, "B9nopuz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>16</v>
       </c>
@@ -5060,7 +5062,7 @@
         <v xml:space="preserve">(16, "B9nopuz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>17</v>
       </c>
@@ -5098,7 +5100,7 @@
         <v xml:space="preserve">(17, "B9nopuz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>18</v>
       </c>
@@ -5136,7 +5138,7 @@
         <v xml:space="preserve">(18, "B9nopuz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>21</v>
       </c>
@@ -5174,7 +5176,7 @@
         <v xml:space="preserve">(21, "B9nopuz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>22</v>
       </c>
@@ -5212,7 +5214,7 @@
         <v xml:space="preserve">(22, "B9nopuz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>23</v>
       </c>
@@ -5250,7 +5252,7 @@
         <v xml:space="preserve">(23, "B9nopuz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>24</v>
       </c>
@@ -5288,7 +5290,7 @@
         <v xml:space="preserve">(24, "B9nopuz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>25</v>
       </c>
@@ -5326,7 +5328,7 @@
         <v xml:space="preserve">(25, "B9nopuz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>26</v>
       </c>
@@ -5364,7 +5366,7 @@
         <v xml:space="preserve">(26, "B9nopuz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>27</v>
       </c>
@@ -5402,7 +5404,7 @@
         <v xml:space="preserve">(27, "B9nopuz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>28</v>
       </c>
@@ -5440,7 +5442,7 @@
         <v xml:space="preserve">(28, "B9nopuz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>31</v>
       </c>
@@ -5478,7 +5480,7 @@
         <v xml:space="preserve">(31, "B9nopuz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>32</v>
       </c>
@@ -5516,7 +5518,7 @@
         <v xml:space="preserve">(32, "B9nopuz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>33</v>
       </c>
@@ -5554,7 +5556,7 @@
         <v xml:space="preserve">(33, "B9nopuz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>34</v>
       </c>
@@ -5592,7 +5594,7 @@
         <v xml:space="preserve">(34, "B9nopuz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>35</v>
       </c>
@@ -5630,7 +5632,7 @@
         <v xml:space="preserve">(35, "B9nopuz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>36</v>
       </c>
@@ -5668,7 +5670,7 @@
         <v xml:space="preserve">(36, "B9nopuz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>37</v>
       </c>
@@ -5706,7 +5708,7 @@
         <v xml:space="preserve">(37, "B9nopuz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>38</v>
       </c>
@@ -5744,7 +5746,7 @@
         <v xml:space="preserve">(38, "B9nopuz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>41</v>
       </c>
@@ -5782,7 +5784,7 @@
         <v xml:space="preserve">(41, "B9nopuz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>42</v>
       </c>
@@ -5820,7 +5822,7 @@
         <v xml:space="preserve">(42, "B9nopuz", 1, 0, 0, 1, 0), </v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>43</v>
       </c>
@@ -5858,7 +5860,7 @@
         <v xml:space="preserve">(43, "B9nopuz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>44</v>
       </c>
@@ -5896,7 +5898,7 @@
         <v xml:space="preserve">(44, "B9nopuz", 0, 0, 1, 1, 0), </v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>45</v>
       </c>
@@ -5934,7 +5936,7 @@
         <v xml:space="preserve">(45, "B9nopuz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>46</v>
       </c>
@@ -5972,7 +5974,7 @@
         <v xml:space="preserve">(46, "B9nopuz", 1, 0, 0, 1, 0), </v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>47</v>
       </c>
@@ -6010,7 +6012,7 @@
         <v xml:space="preserve">(47, "B9nopuz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>48</v>
       </c>
@@ -6048,7 +6050,7 @@
         <v xml:space="preserve">(48, "B9nopuz", 0, 0, 1, 1, 0), </v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>51</v>
       </c>
@@ -6086,7 +6088,7 @@
         <v xml:space="preserve">(51, "B9nopuz", 1, 0, 0, 1, 0), </v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>52</v>
       </c>
@@ -6124,7 +6126,7 @@
         <v xml:space="preserve">(52, "B9nopuz", 1, 0, 0, 1, 0), </v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>53</v>
       </c>
@@ -6162,7 +6164,7 @@
         <v xml:space="preserve">(53, "B9nopuz", 0, 0, 1, 1, 0), </v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>54</v>
       </c>
@@ -6200,7 +6202,7 @@
         <v xml:space="preserve">(54, "B9nopuz", 0, 0, 1, 1, 0), </v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>55</v>
       </c>
@@ -6238,7 +6240,7 @@
         <v xml:space="preserve">(55, "B9nopuz", 1, 0, 0, 1, 0), </v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>56</v>
       </c>
@@ -6276,7 +6278,7 @@
         <v xml:space="preserve">(56, "B9nopuz", 1, 0, 0, 1, 0), </v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>57</v>
       </c>
@@ -6314,7 +6316,7 @@
         <v xml:space="preserve">(57, "B9nopuz", 0, 0, 1, 1, 0), </v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>58</v>
       </c>
@@ -6352,7 +6354,7 @@
         <v xml:space="preserve">(58, "B9nopuz", 0, 0, 1, 1, 0), </v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>61</v>
       </c>
@@ -6390,7 +6392,7 @@
         <v xml:space="preserve">(61, "B9nopuz", 1, 0, 0, 1, 0), </v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>62</v>
       </c>
@@ -6428,7 +6430,7 @@
         <v xml:space="preserve">(62, "B9nopuz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>63</v>
       </c>
@@ -6466,7 +6468,7 @@
         <v xml:space="preserve">(63, "B9nopuz", 0, 0, 1, 1, 0), </v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>64</v>
       </c>
@@ -6504,7 +6506,7 @@
         <v xml:space="preserve">(64, "B9nopuz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>65</v>
       </c>
@@ -6542,7 +6544,7 @@
         <v xml:space="preserve">(65, "B9nopuz", 1, 0, 0, 1, 0), </v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>66</v>
       </c>
@@ -6580,7 +6582,7 @@
         <v xml:space="preserve">(66, "B9nopuz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>67</v>
       </c>
@@ -6618,7 +6620,7 @@
         <v xml:space="preserve">(67, "B9nopuz", 0, 0, 1, 1, 0), </v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>68</v>
       </c>
@@ -6656,7 +6658,7 @@
         <v xml:space="preserve">(68, "B9nopuz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>71</v>
       </c>
@@ -6694,7 +6696,7 @@
         <v xml:space="preserve">(71, "B9nopuz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>72</v>
       </c>
@@ -6732,7 +6734,7 @@
         <v xml:space="preserve">(72, "B9nopuz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>73</v>
       </c>
@@ -6770,7 +6772,7 @@
         <v xml:space="preserve">(73, "B9nopuz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>74</v>
       </c>
@@ -6808,7 +6810,7 @@
         <v xml:space="preserve">(74, "B9nopuz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>75</v>
       </c>
@@ -6846,7 +6848,7 @@
         <v xml:space="preserve">(75, "B9nopuz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>76</v>
       </c>
@@ -6884,7 +6886,7 @@
         <v xml:space="preserve">(76, "B9nopuz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>77</v>
       </c>
@@ -6922,7 +6924,7 @@
         <v xml:space="preserve">(77, "B9nopuz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>78</v>
       </c>
@@ -6960,7 +6962,7 @@
         <v xml:space="preserve">(78, "B9nopuz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>81</v>
       </c>
@@ -6998,7 +7000,7 @@
         <v xml:space="preserve">(81, "B9nopuz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>82</v>
       </c>
@@ -7036,7 +7038,7 @@
         <v xml:space="preserve">(82, "B9nopuz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>83</v>
       </c>
@@ -7074,7 +7076,7 @@
         <v xml:space="preserve">(83, "B9nopuz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>84</v>
       </c>
@@ -7112,7 +7114,7 @@
         <v xml:space="preserve">(84, "B9nopuz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>85</v>
       </c>
@@ -7150,7 +7152,7 @@
         <v xml:space="preserve">(85, "B9nopuz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>86</v>
       </c>
@@ -7188,7 +7190,7 @@
         <v xml:space="preserve">(86, "B9nopuz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>87</v>
       </c>
@@ -7226,7 +7228,7 @@
         <v xml:space="preserve">(87, "B9nopuz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>88</v>
       </c>
@@ -7264,7 +7266,7 @@
         <v xml:space="preserve">(88, "B9nopuz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>91</v>
       </c>
@@ -7302,7 +7304,7 @@
         <v xml:space="preserve">(91, "B9nopuz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>92</v>
       </c>
@@ -7340,7 +7342,7 @@
         <v xml:space="preserve">(92, "B9nopuz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>93</v>
       </c>
@@ -7378,7 +7380,7 @@
         <v xml:space="preserve">(93, "B9nopuz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>94</v>
       </c>
@@ -7416,7 +7418,7 @@
         <v xml:space="preserve">(94, "B9nopuz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>95</v>
       </c>
@@ -7454,7 +7456,7 @@
         <v xml:space="preserve">(95, "B9nopuz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>96</v>
       </c>
@@ -7492,7 +7494,7 @@
         <v xml:space="preserve">(96, "B9nopuz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>97</v>
       </c>
@@ -7530,7 +7532,7 @@
         <v xml:space="preserve">(97, "B9nopuz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>98</v>
       </c>
@@ -7581,12 +7583,12 @@
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="8" max="8" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -7612,7 +7614,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>11</v>
       </c>
@@ -7643,7 +7645,7 @@
         <v xml:space="preserve">(11, "B7bnopuz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>12</v>
       </c>
@@ -7658,23 +7660,23 @@
         <v>1</v>
       </c>
       <c r="H3" t="str">
-        <f t="shared" ref="H3:H61" si="1">_xlfn.CONCAT("(",A3)</f>
+        <f t="shared" ref="H3:H59" si="1">_xlfn.CONCAT("(",A3)</f>
         <v>(12</v>
       </c>
       <c r="I3" t="str">
-        <f t="shared" ref="I3:I61" si="2">_xlfn.CONCAT(H3,", ",$I$1,"B7bnopuz",$I$1)</f>
+        <f t="shared" ref="I3:I59" si="2">_xlfn.CONCAT(H3,", ",$I$1,"B7bnopuz",$I$1)</f>
         <v>(12, "B7bnopuz"</v>
       </c>
       <c r="J3" t="str">
-        <f t="shared" ref="J3:J61" si="3">_xlfn.CONCAT(I3,", ",D3,", ",C3)</f>
+        <f t="shared" ref="J3:J59" si="3">_xlfn.CONCAT(I3,", ",D3,", ",C3)</f>
         <v>(12, "B7bnopuz", 1, 0</v>
       </c>
       <c r="K3" t="str">
-        <f t="shared" ref="K3:K61" si="4">_xlfn.CONCAT(J3,", ",B3,", 0, 0), ")</f>
+        <f t="shared" ref="K3:K59" si="4">_xlfn.CONCAT(J3,", ",B3,", 0, 0), ")</f>
         <v xml:space="preserve">(12, "B7bnopuz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>13</v>
       </c>
@@ -7705,7 +7707,7 @@
         <v xml:space="preserve">(13, "B7bnopuz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>14</v>
       </c>
@@ -7736,7 +7738,7 @@
         <v xml:space="preserve">(14, "B7bnopuz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>15</v>
       </c>
@@ -7769,7 +7771,7 @@
         <v xml:space="preserve">(15, "B7bnopuz", 1, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>16</v>
       </c>
@@ -7800,7 +7802,7 @@
         <v xml:space="preserve">(16, "B7bnopuz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>17</v>
       </c>
@@ -7833,7 +7835,7 @@
         <v xml:space="preserve">(17, "B7bnopuz", 1, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>18</v>
       </c>
@@ -7864,7 +7866,7 @@
         <v xml:space="preserve">(18, "B7bnopuz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>21</v>
       </c>
@@ -7895,7 +7897,7 @@
         <v xml:space="preserve">(21, "B7bnopuz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>22</v>
       </c>
@@ -7926,7 +7928,7 @@
         <v xml:space="preserve">(22, "B7bnopuz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>23</v>
       </c>
@@ -7957,7 +7959,7 @@
         <v xml:space="preserve">(23, "B7bnopuz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>24</v>
       </c>
@@ -7988,7 +7990,7 @@
         <v xml:space="preserve">(24, "B7bnopuz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>25</v>
       </c>
@@ -8019,7 +8021,7 @@
         <v xml:space="preserve">(25, "B7bnopuz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>26</v>
       </c>
@@ -8050,7 +8052,7 @@
         <v xml:space="preserve">(26, "B7bnopuz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>27</v>
       </c>
@@ -8081,7 +8083,7 @@
         <v xml:space="preserve">(27, "B7bnopuz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>28</v>
       </c>
@@ -8112,7 +8114,7 @@
         <v xml:space="preserve">(28, "B7bnopuz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>31</v>
       </c>
@@ -8143,7 +8145,7 @@
         <v xml:space="preserve">(31, "B7bnopuz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>32</v>
       </c>
@@ -8174,7 +8176,7 @@
         <v xml:space="preserve">(32, "B7bnopuz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>33</v>
       </c>
@@ -8205,7 +8207,7 @@
         <v xml:space="preserve">(33, "B7bnopuz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>34</v>
       </c>
@@ -8236,7 +8238,7 @@
         <v xml:space="preserve">(34, "B7bnopuz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>35</v>
       </c>
@@ -8267,7 +8269,7 @@
         <v xml:space="preserve">(35, "B7bnopuz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>36</v>
       </c>
@@ -8298,7 +8300,7 @@
         <v xml:space="preserve">(36, "B7bnopuz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>37</v>
       </c>
@@ -8329,7 +8331,7 @@
         <v xml:space="preserve">(37, "B7bnopuz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>38</v>
       </c>
@@ -8360,7 +8362,7 @@
         <v xml:space="preserve">(38, "B7bnopuz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>41</v>
       </c>
@@ -8391,7 +8393,7 @@
         <v xml:space="preserve">(41, "B7bnopuz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>42</v>
       </c>
@@ -8422,7 +8424,7 @@
         <v xml:space="preserve">(42, "B7bnopuz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>43</v>
       </c>
@@ -8453,7 +8455,7 @@
         <v xml:space="preserve">(43, "B7bnopuz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>44</v>
       </c>
@@ -8484,7 +8486,7 @@
         <v xml:space="preserve">(44, "B7bnopuz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>45</v>
       </c>
@@ -8515,7 +8517,7 @@
         <v xml:space="preserve">(45, "B7bnopuz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>46</v>
       </c>
@@ -8546,7 +8548,7 @@
         <v xml:space="preserve">(46, "B7bnopuz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>47</v>
       </c>
@@ -8577,7 +8579,7 @@
         <v xml:space="preserve">(47, "B7bnopuz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>48</v>
       </c>
@@ -8608,7 +8610,7 @@
         <v xml:space="preserve">(48, "B7bnopuz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>51</v>
       </c>
@@ -8639,7 +8641,7 @@
         <v xml:space="preserve">(51, "B7bnopuz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>52</v>
       </c>
@@ -8670,7 +8672,7 @@
         <v xml:space="preserve">(52, "B7bnopuz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>53</v>
       </c>
@@ -8701,7 +8703,7 @@
         <v xml:space="preserve">(53, "B7bnopuz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>54</v>
       </c>
@@ -8732,7 +8734,7 @@
         <v xml:space="preserve">(54, "B7bnopuz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>55</v>
       </c>
@@ -8763,7 +8765,7 @@
         <v xml:space="preserve">(55, "B7bnopuz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>56</v>
       </c>
@@ -8794,7 +8796,7 @@
         <v xml:space="preserve">(56, "B7bnopuz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>57</v>
       </c>
@@ -8825,7 +8827,7 @@
         <v xml:space="preserve">(57, "B7bnopuz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>58</v>
       </c>
@@ -8856,7 +8858,7 @@
         <v xml:space="preserve">(58, "B7bnopuz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>61</v>
       </c>
@@ -8887,7 +8889,7 @@
         <v xml:space="preserve">(61, "B7bnopuz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>62</v>
       </c>
@@ -8918,7 +8920,7 @@
         <v xml:space="preserve">(62, "B7bnopuz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>63</v>
       </c>
@@ -8949,7 +8951,7 @@
         <v xml:space="preserve">(63, "B7bnopuz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>64</v>
       </c>
@@ -8980,7 +8982,7 @@
         <v xml:space="preserve">(64, "B7bnopuz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>65</v>
       </c>
@@ -9011,7 +9013,7 @@
         <v xml:space="preserve">(65, "B7bnopuz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>66</v>
       </c>
@@ -9042,7 +9044,7 @@
         <v xml:space="preserve">(66, "B7bnopuz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>67</v>
       </c>
@@ -9073,7 +9075,7 @@
         <v xml:space="preserve">(67, "B7bnopuz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>68</v>
       </c>
@@ -9104,7 +9106,7 @@
         <v xml:space="preserve">(68, "B7bnopuz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>71</v>
       </c>
@@ -9135,7 +9137,7 @@
         <v xml:space="preserve">(71, "B7bnopuz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>72</v>
       </c>
@@ -9166,7 +9168,7 @@
         <v xml:space="preserve">(72, "B7bnopuz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>73</v>
       </c>
@@ -9197,7 +9199,7 @@
         <v xml:space="preserve">(73, "B7bnopuz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>74</v>
       </c>
@@ -9228,7 +9230,7 @@
         <v xml:space="preserve">(74, "B7bnopuz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>75</v>
       </c>
@@ -9259,7 +9261,7 @@
         <v xml:space="preserve">(75, "B7bnopuz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>76</v>
       </c>
@@ -9290,7 +9292,7 @@
         <v xml:space="preserve">(76, "B7bnopuz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>77</v>
       </c>
@@ -9321,7 +9323,7 @@
         <v xml:space="preserve">(77, "B7bnopuz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>78</v>
       </c>
@@ -9352,7 +9354,7 @@
         <v xml:space="preserve">(78, "B7bnopuz", 0, 0, 1, 0, 0), </v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>81</v>
       </c>
@@ -9383,7 +9385,7 @@
         <v xml:space="preserve">(81, "B7bnopuz", 1, 0, 0, 0, 0), </v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>83</v>
       </c>
@@ -9427,12 +9429,12 @@
       <selection activeCell="K1" sqref="K1:K1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="8" max="8" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -9458,7 +9460,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>11</v>
       </c>
@@ -9491,7 +9493,7 @@
         <v xml:space="preserve">(11, "A9nouz", 0, 0, 1, 0, 1), </v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>12</v>
       </c>
@@ -9508,23 +9510,23 @@
         <v>1</v>
       </c>
       <c r="H3" t="str">
-        <f t="shared" ref="H3:H61" si="0">_xlfn.CONCAT("(",A3)</f>
+        <f t="shared" ref="H3:H55" si="0">_xlfn.CONCAT("(",A3)</f>
         <v>(12</v>
       </c>
       <c r="I3" t="str">
-        <f t="shared" ref="I3:I59" si="1">_xlfn.CONCAT(H3,", ",$I$1,"A9nouz",$I$1)</f>
+        <f t="shared" ref="I3:I55" si="1">_xlfn.CONCAT(H3,", ",$I$1,"A9nouz",$I$1)</f>
         <v>(12, "A9nouz"</v>
       </c>
       <c r="J3" t="str">
-        <f t="shared" ref="J3:J59" si="2">_xlfn.CONCAT(I3,", ",D3,", ",C3)</f>
+        <f t="shared" ref="J3:J55" si="2">_xlfn.CONCAT(I3,", ",D3,", ",C3)</f>
         <v>(12, "A9nouz", 0, 0</v>
       </c>
       <c r="K3" t="str">
-        <f t="shared" ref="K3:K59" si="3">_xlfn.CONCAT(J3,", ",B3,", 0, 1), ")</f>
+        <f t="shared" ref="K3:K55" si="3">_xlfn.CONCAT(J3,", ",B3,", 0, 1), ")</f>
         <v xml:space="preserve">(12, "A9nouz", 0, 0, 1, 0, 1), </v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>13</v>
       </c>
@@ -9557,7 +9559,7 @@
         <v xml:space="preserve">(13, "A9nouz", 0, 1, 0, 0, 1), </v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>14</v>
       </c>
@@ -9590,7 +9592,7 @@
         <v xml:space="preserve">(14, "A9nouz", 0, 1, 0, 0, 1), </v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>15</v>
       </c>
@@ -9623,7 +9625,7 @@
         <v xml:space="preserve">(15, "A9nouz", 1, 0, 0, 0, 1), </v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>16</v>
       </c>
@@ -9656,7 +9658,7 @@
         <v xml:space="preserve">(16, "A9nouz", 1, 0, 0, 0, 1), </v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>21</v>
       </c>
@@ -9689,7 +9691,7 @@
         <v xml:space="preserve">(21, "A9nouz", 0, 0, 1, 0, 1), </v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>22</v>
       </c>
@@ -9722,7 +9724,7 @@
         <v xml:space="preserve">(22, "A9nouz", 0, 0, 1, 0, 1), </v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>23</v>
       </c>
@@ -9755,7 +9757,7 @@
         <v xml:space="preserve">(23, "A9nouz", 0, 1, 0, 0, 1), </v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>24</v>
       </c>
@@ -9788,7 +9790,7 @@
         <v xml:space="preserve">(24, "A9nouz", 0, 1, 0, 0, 1), </v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>25</v>
       </c>
@@ -9821,7 +9823,7 @@
         <v xml:space="preserve">(25, "A9nouz", 1, 0, 0, 0, 1), </v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>26</v>
       </c>
@@ -9854,7 +9856,7 @@
         <v xml:space="preserve">(26, "A9nouz", 1, 0, 0, 0, 1), </v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>31</v>
       </c>
@@ -9887,7 +9889,7 @@
         <v xml:space="preserve">(31, "A9nouz", 0, 0, 1, 0, 1), </v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>32</v>
       </c>
@@ -9920,7 +9922,7 @@
         <v xml:space="preserve">(32, "A9nouz", 0, 0, 1, 0, 1), </v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>33</v>
       </c>
@@ -9953,7 +9955,7 @@
         <v xml:space="preserve">(33, "A9nouz", 0, 1, 0, 0, 1), </v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>34</v>
       </c>
@@ -9986,7 +9988,7 @@
         <v xml:space="preserve">(34, "A9nouz", 0, 1, 0, 0, 1), </v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>35</v>
       </c>
@@ -10019,7 +10021,7 @@
         <v xml:space="preserve">(35, "A9nouz", 1, 0, 0, 0, 1), </v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>36</v>
       </c>
@@ -10052,7 +10054,7 @@
         <v xml:space="preserve">(36, "A9nouz", 1, 0, 0, 0, 1), </v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>41</v>
       </c>
@@ -10085,7 +10087,7 @@
         <v xml:space="preserve">(41, "A9nouz", 0, 0, 1, 0, 1), </v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>42</v>
       </c>
@@ -10118,7 +10120,7 @@
         <v xml:space="preserve">(42, "A9nouz", 0, 0, 1, 0, 1), </v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>43</v>
       </c>
@@ -10151,7 +10153,7 @@
         <v xml:space="preserve">(43, "A9nouz", 0, 1, 0, 0, 1), </v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>44</v>
       </c>
@@ -10184,7 +10186,7 @@
         <v xml:space="preserve">(44, "A9nouz", 0, 1, 0, 0, 1), </v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>45</v>
       </c>
@@ -10217,7 +10219,7 @@
         <v xml:space="preserve">(45, "A9nouz", 1, 0, 0, 0, 1), </v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>46</v>
       </c>
@@ -10250,7 +10252,7 @@
         <v xml:space="preserve">(46, "A9nouz", 1, 0, 0, 0, 1), </v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>51</v>
       </c>
@@ -10283,7 +10285,7 @@
         <v xml:space="preserve">(51, "A9nouz", 0, 0, 1, 0, 1), </v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>52</v>
       </c>
@@ -10316,7 +10318,7 @@
         <v xml:space="preserve">(52, "A9nouz", 0, 0, 1, 0, 1), </v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>53</v>
       </c>
@@ -10349,7 +10351,7 @@
         <v xml:space="preserve">(53, "A9nouz", 0, 1, 0, 0, 1), </v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>54</v>
       </c>
@@ -10382,7 +10384,7 @@
         <v xml:space="preserve">(54, "A9nouz", 0, 1, 0, 0, 1), </v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>55</v>
       </c>
@@ -10415,7 +10417,7 @@
         <v xml:space="preserve">(55, "A9nouz", 1, 0, 0, 0, 1), </v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>56</v>
       </c>
@@ -10448,7 +10450,7 @@
         <v xml:space="preserve">(56, "A9nouz", 1, 0, 0, 0, 1), </v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>61</v>
       </c>
@@ -10481,7 +10483,7 @@
         <v xml:space="preserve">(61, "A9nouz", 0, 0, 1, 0, 1), </v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>62</v>
       </c>
@@ -10514,7 +10516,7 @@
         <v xml:space="preserve">(62, "A9nouz", 0, 0, 1, 0, 1), </v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>63</v>
       </c>
@@ -10547,7 +10549,7 @@
         <v xml:space="preserve">(63, "A9nouz", 0, 1, 0, 0, 1), </v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>64</v>
       </c>
@@ -10580,7 +10582,7 @@
         <v xml:space="preserve">(64, "A9nouz", 0, 1, 0, 0, 1), </v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>65</v>
       </c>
@@ -10613,7 +10615,7 @@
         <v xml:space="preserve">(65, "A9nouz", 1, 0, 0, 0, 1), </v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>66</v>
       </c>
@@ -10646,7 +10648,7 @@
         <v xml:space="preserve">(66, "A9nouz", 1, 0, 0, 0, 1), </v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>71</v>
       </c>
@@ -10679,7 +10681,7 @@
         <v xml:space="preserve">(71, "A9nouz", 0, 0, 1, 0, 1), </v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>72</v>
       </c>
@@ -10712,7 +10714,7 @@
         <v xml:space="preserve">(72, "A9nouz", 0, 0, 1, 0, 1), </v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>73</v>
       </c>
@@ -10745,7 +10747,7 @@
         <v xml:space="preserve">(73, "A9nouz", 0, 1, 0, 0, 1), </v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>74</v>
       </c>
@@ -10778,7 +10780,7 @@
         <v xml:space="preserve">(74, "A9nouz", 0, 1, 0, 0, 1), </v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>75</v>
       </c>
@@ -10811,7 +10813,7 @@
         <v xml:space="preserve">(75, "A9nouz", 1, 0, 0, 0, 1), </v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>76</v>
       </c>
@@ -10844,7 +10846,7 @@
         <v xml:space="preserve">(76, "A9nouz", 1, 0, 0, 0, 1), </v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>81</v>
       </c>
@@ -10877,7 +10879,7 @@
         <v xml:space="preserve">(81, "A9nouz", 0, 0, 1, 0, 1), </v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>82</v>
       </c>
@@ -10910,7 +10912,7 @@
         <v xml:space="preserve">(82, "A9nouz", 0, 0, 1, 0, 1), </v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>83</v>
       </c>
@@ -10943,7 +10945,7 @@
         <v xml:space="preserve">(83, "A9nouz", 0, 1, 0, 0, 1), </v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>84</v>
       </c>
@@ -10976,7 +10978,7 @@
         <v xml:space="preserve">(84, "A9nouz", 0, 1, 0, 0, 1), </v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>85</v>
       </c>
@@ -11009,7 +11011,7 @@
         <v xml:space="preserve">(85, "A9nouz", 1, 0, 0, 0, 1), </v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>86</v>
       </c>
@@ -11042,7 +11044,7 @@
         <v xml:space="preserve">(86, "A9nouz", 1, 0, 0, 0, 1), </v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>91</v>
       </c>
@@ -11075,7 +11077,7 @@
         <v xml:space="preserve">(91, "A9nouz", 0, 0, 1, 0, 1), </v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>92</v>
       </c>
@@ -11108,7 +11110,7 @@
         <v xml:space="preserve">(92, "A9nouz", 0, 0, 1, 0, 1), </v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>93</v>
       </c>
@@ -11141,7 +11143,7 @@
         <v xml:space="preserve">(93, "A9nouz", 0, 1, 0, 0, 1), </v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>94</v>
       </c>
@@ -11174,7 +11176,7 @@
         <v xml:space="preserve">(94, "A9nouz", 0, 1, 0, 0, 1), </v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>95</v>
       </c>
@@ -11207,7 +11209,7 @@
         <v xml:space="preserve">(95, "A9nouz", 1, 0, 0, 0, 1), </v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>96</v>
       </c>

</xml_diff>

<commit_message>
Deleted TripID from TrainSets
</commit_message>
<xml_diff>
--- a/System_Biletow/cars-and-seats.xlsx
+++ b/System_Biletow/cars-and-seats.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marta\source\repos\System_Biletow\System_Biletow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38B949AD-8E90-4B77-83C6-67734D51BB15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACBFB2E2-090D-4C1C-BAD4-BC9550AF3A9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="11370" activeTab="1" xr2:uid="{0AE42409-A18E-481D-BAD6-AC22FA644729}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{0AE42409-A18E-481D-BAD6-AC22FA644729}"/>
   </bookViews>
   <sheets>
     <sheet name="TrainSets" sheetId="1" r:id="rId1"/>
@@ -469,7 +469,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48174A8D-7CBB-4DEA-BA67-C42F3F48131F}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
@@ -498,16 +498,16 @@
         <v>2</v>
       </c>
       <c r="C2" t="str">
-        <f>_xlfn.CONCAT("(2, ",$C$1,"IC 8306/7",$C$1,", ")</f>
-        <v xml:space="preserve">(2, "IC 8306/7", </v>
+        <f>_xlfn.CONCAT("(",$C$1,"IC 3806/7",$C$1,", ")</f>
+        <v xml:space="preserve">("IC 3806/7", </v>
       </c>
       <c r="D2" t="str">
         <f>_xlfn.CONCAT(C2,$C$1,B2,$C$1,", ")</f>
-        <v xml:space="preserve">(2, "IC 8306/7", "B10nouz", </v>
+        <v xml:space="preserve">("IC 3806/7", "B10nouz", </v>
       </c>
       <c r="E2" t="str">
         <f>_xlfn.CONCAT(D2,A2,"), ")</f>
-        <v xml:space="preserve">(2, "IC 8306/7", "B10nouz", 18), </v>
+        <v xml:space="preserve">("IC 3806/7", "B10nouz", 18), </v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -518,16 +518,16 @@
         <v>3</v>
       </c>
       <c r="C3" t="str">
-        <f t="shared" ref="C3:C9" si="0">_xlfn.CONCAT("(2, ",$C$1,"IC 8306/7",$C$1,", ")</f>
-        <v xml:space="preserve">(2, "IC 8306/7", </v>
+        <f t="shared" ref="C3:C9" si="0">_xlfn.CONCAT("(",$C$1,"IC 3806/7",$C$1,", ")</f>
+        <v xml:space="preserve">("IC 3806/7", </v>
       </c>
       <c r="D3" t="str">
         <f t="shared" ref="D3:D9" si="1">_xlfn.CONCAT(C3,$C$1,B3,$C$1,", ")</f>
-        <v xml:space="preserve">(2, "IC 8306/7", "B9nopuvz", </v>
+        <v xml:space="preserve">("IC 3806/7", "B9nopuvz", </v>
       </c>
       <c r="E3" t="str">
         <f t="shared" ref="E3:E9" si="2">_xlfn.CONCAT(D3,A3,"), ")</f>
-        <v xml:space="preserve">(2, "IC 8306/7", "B9nopuvz", 17), </v>
+        <v xml:space="preserve">("IC 3806/7", "B9nopuvz", 17), </v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -539,15 +539,15 @@
       </c>
       <c r="C4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">(2, "IC 8306/7", </v>
+        <v xml:space="preserve">("IC 3806/7", </v>
       </c>
       <c r="D4" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">(2, "IC 8306/7", "B9nopuz", </v>
+        <v xml:space="preserve">("IC 3806/7", "B9nopuz", </v>
       </c>
       <c r="E4" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">(2, "IC 8306/7", "B9nopuz", 16), </v>
+        <v xml:space="preserve">("IC 3806/7", "B9nopuz", 16), </v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -559,15 +559,15 @@
       </c>
       <c r="C5" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">(2, "IC 8306/7", </v>
+        <v xml:space="preserve">("IC 3806/7", </v>
       </c>
       <c r="D5" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">(2, "IC 8306/7", "B9nopuz", </v>
+        <v xml:space="preserve">("IC 3806/7", "B9nopuz", </v>
       </c>
       <c r="E5" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">(2, "IC 8306/7", "B9nopuz", 15), </v>
+        <v xml:space="preserve">("IC 3806/7", "B9nopuz", 15), </v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -579,15 +579,15 @@
       </c>
       <c r="C6" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">(2, "IC 8306/7", </v>
+        <v xml:space="preserve">("IC 3806/7", </v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">(2, "IC 8306/7", "B10nouz", </v>
+        <v xml:space="preserve">("IC 3806/7", "B10nouz", </v>
       </c>
       <c r="E6" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">(2, "IC 8306/7", "B10nouz", 14), </v>
+        <v xml:space="preserve">("IC 3806/7", "B10nouz", 14), </v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -599,15 +599,15 @@
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">(2, "IC 8306/7", </v>
+        <v xml:space="preserve">("IC 3806/7", </v>
       </c>
       <c r="D7" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">(2, "IC 8306/7", "B7bnopuz", </v>
+        <v xml:space="preserve">("IC 3806/7", "B7bnopuz", </v>
       </c>
       <c r="E7" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">(2, "IC 8306/7", "B7bnopuz", 13), </v>
+        <v xml:space="preserve">("IC 3806/7", "B7bnopuz", 13), </v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -619,15 +619,15 @@
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">(2, "IC 8306/7", </v>
+        <v xml:space="preserve">("IC 3806/7", </v>
       </c>
       <c r="D8" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">(2, "IC 8306/7", "WRnouz", </v>
+        <v xml:space="preserve">("IC 3806/7", "WRnouz", </v>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">(2, "IC 8306/7", "WRnouz", 12), </v>
+        <v xml:space="preserve">("IC 3806/7", "WRnouz", 12), </v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -639,15 +639,15 @@
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">(2, "IC 8306/7", </v>
+        <v xml:space="preserve">("IC 3806/7", </v>
       </c>
       <c r="D9" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">(2, "IC 8306/7", "A9nouz", </v>
+        <v xml:space="preserve">("IC 3806/7", "A9nouz", </v>
       </c>
       <c r="E9" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">(2, "IC 8306/7", "A9nouz", 11), </v>
+        <v xml:space="preserve">("IC 3806/7", "A9nouz", 11), </v>
       </c>
     </row>
   </sheetData>
@@ -659,7 +659,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C9B2C30-95FD-4C71-961A-ECB353A345A8}">
   <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>

</xml_diff>